<commit_message>
Heavy Fixed wing loc and planes added
Update to USA, Russia, China
</commit_message>
<xml_diff>
--- a/Modding resources/Equipment codes for OOBs.xlsx
+++ b/Modding resources/Equipment codes for OOBs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="476">
   <si>
     <t>Equipment Code</t>
   </si>
@@ -1303,9 +1303,6 @@
     <t>Required tech for 4.5 Gen and 5th Gen Strike Fighters</t>
   </si>
   <si>
-    <t>The rest is work in progress. Missing Light Jets, Helicopters, Bombers and transport planes, and all ships. Note that all land equipment is included.</t>
-  </si>
-  <si>
     <t>L_Strike_fighter_equipment_1</t>
   </si>
   <si>
@@ -1324,10 +1321,106 @@
     <t>L_Strike_fighter3</t>
   </si>
   <si>
+    <t>early_bomber</t>
+  </si>
+  <si>
+    <t>Required for strat bomb, tra plane, maritime patrol</t>
+  </si>
+  <si>
+    <t>strategic_bomber_equipment_1</t>
+  </si>
+  <si>
+    <t>strategic_bomber1</t>
+  </si>
+  <si>
+    <t>strategic_bomber_equipment_2</t>
+  </si>
+  <si>
+    <t>strategic_bomber2</t>
+  </si>
+  <si>
+    <t>strategic_bomber_equipment_3</t>
+  </si>
+  <si>
+    <t>strategic_bomber3</t>
+  </si>
+  <si>
+    <t>strategic_bomber_equipment_4</t>
+  </si>
+  <si>
+    <t>strategic_bomber4</t>
+  </si>
+  <si>
+    <t>B-2</t>
+  </si>
+  <si>
+    <t>transport_plane_equipment_1</t>
+  </si>
+  <si>
+    <t>transport_plane1</t>
+  </si>
+  <si>
+    <t>transport_plane_equipment_2</t>
+  </si>
+  <si>
+    <t>transport_plane2</t>
+  </si>
+  <si>
+    <t>transport_plane_equipment_3</t>
+  </si>
+  <si>
+    <t>transport_plane3</t>
+  </si>
+  <si>
+    <t>transport_plane_equipment_4</t>
+  </si>
+  <si>
+    <t>transport_plane4</t>
+  </si>
+  <si>
+    <t>nav_plane_equipment_1</t>
+  </si>
+  <si>
+    <t>naval_plane1</t>
+  </si>
+  <si>
+    <t>nav_plane_equipment_2</t>
+  </si>
+  <si>
+    <t>naval_plane2</t>
+  </si>
+  <si>
+    <t>nav_plane_equipment_3</t>
+  </si>
+  <si>
+    <t>naval_plane3</t>
+  </si>
+  <si>
+    <t>nav_plane_equipment_4</t>
+  </si>
+  <si>
+    <t>naval_plane4</t>
+  </si>
+  <si>
+    <t>CAS_equipment_1</t>
+  </si>
+  <si>
+    <t>cas1</t>
+  </si>
+  <si>
+    <t>CAS_equipment_2</t>
+  </si>
+  <si>
+    <t>cas2</t>
+  </si>
+  <si>
+    <t>CAS_equipment_3</t>
+  </si>
+  <si>
+    <t>cas3</t>
+  </si>
+  <si>
     <t>early_helicopter</t>
-  </si>
-  <si>
-    <t>Transport Helicopter</t>
   </si>
   <si>
     <t>attack_helicopter_equipment_1</t>
@@ -1478,21 +1571,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G192"/>
+  <dimension ref="A1:G208"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="510" topLeftCell="A109" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="510" topLeftCell="A172" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D125" activeCellId="0" sqref="D125"/>
+      <selection pane="bottomLeft" activeCell="C200" activeCellId="0" sqref="C200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3804,132 +3898,325 @@
       <c r="D175" s="3"/>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="1" t="s">
+      <c r="A176" s="0" t="s">
         <v>427</v>
       </c>
-      <c r="C176" s="5"/>
+      <c r="B176" s="0" t="s">
+        <v>428</v>
+      </c>
+      <c r="C176" s="5" t="n">
+        <v>1975</v>
+      </c>
       <c r="D176" s="3"/>
     </row>
+    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="0" t="s">
+        <v>429</v>
+      </c>
+      <c r="B177" s="0" t="s">
+        <v>430</v>
+      </c>
+      <c r="C177" s="5" t="n">
+        <v>1995</v>
+      </c>
+      <c r="D177" s="3"/>
+    </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C178" s="5"/>
+      <c r="A178" s="0" t="s">
+        <v>431</v>
+      </c>
+      <c r="B178" s="0" t="s">
+        <v>432</v>
+      </c>
+      <c r="C178" s="5" t="n">
+        <v>2015</v>
+      </c>
       <c r="D178" s="3"/>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="0" t="s">
-        <v>428</v>
-      </c>
-      <c r="B179" s="0" t="s">
-        <v>429</v>
-      </c>
-      <c r="C179" s="5" t="n">
+      <c r="C179" s="5"/>
+      <c r="D179" s="3"/>
+    </row>
+    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B180" s="0" t="s">
+        <v>433</v>
+      </c>
+      <c r="C180" s="5" t="n">
+        <v>1965</v>
+      </c>
+      <c r="D180" s="3" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C181" s="5"/>
+      <c r="D181" s="3"/>
+    </row>
+    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="0" t="s">
+        <v>435</v>
+      </c>
+      <c r="B182" s="0" t="s">
+        <v>436</v>
+      </c>
+      <c r="C182" s="5" t="n">
+        <v>1965</v>
+      </c>
+      <c r="D182" s="3"/>
+    </row>
+    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="0" t="s">
+        <v>437</v>
+      </c>
+      <c r="B183" s="0" t="s">
+        <v>438</v>
+      </c>
+      <c r="C183" s="5" t="n">
         <v>1975</v>
       </c>
-      <c r="D179" s="3"/>
-    </row>
-    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="0" t="s">
-        <v>430</v>
-      </c>
-      <c r="B180" s="0" t="s">
-        <v>431</v>
-      </c>
-      <c r="C180" s="5" t="n">
-        <v>1995</v>
-      </c>
-      <c r="D180" s="3"/>
-    </row>
-    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="0" t="s">
-        <v>432</v>
-      </c>
-      <c r="B181" s="0" t="s">
-        <v>433</v>
-      </c>
-      <c r="C181" s="5" t="n">
-        <v>2015</v>
-      </c>
-      <c r="D181" s="3"/>
-    </row>
-    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C182" s="5"/>
-      <c r="D182" s="3"/>
-    </row>
-    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C183" s="5"/>
       <c r="D183" s="3"/>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C184" s="5"/>
+      <c r="A184" s="0" t="s">
+        <v>439</v>
+      </c>
+      <c r="B184" s="0" t="s">
+        <v>440</v>
+      </c>
+      <c r="C184" s="5" t="n">
+        <v>1985</v>
+      </c>
       <c r="D184" s="3"/>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
-        <v>434</v>
+        <v>441</v>
+      </c>
+      <c r="B185" s="0" t="s">
+        <v>442</v>
       </c>
       <c r="C185" s="5" t="n">
-        <v>1965</v>
-      </c>
-      <c r="D185" s="3" t="s">
-        <v>435</v>
+        <v>2015</v>
+      </c>
+      <c r="D185" s="3"/>
+      <c r="E185" s="0" t="s">
+        <v>443</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A186" s="0" t="s">
-        <v>436</v>
-      </c>
-      <c r="C186" s="5" t="n">
-        <v>1965</v>
-      </c>
-      <c r="D186" s="3" t="s">
-        <v>437</v>
-      </c>
+      <c r="C186" s="5"/>
+      <c r="D186" s="3"/>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
-        <v>438</v>
+        <v>444</v>
+      </c>
+      <c r="B187" s="0" t="s">
+        <v>445</v>
       </c>
       <c r="C187" s="5" t="n">
-        <v>1985</v>
+        <v>1965</v>
       </c>
       <c r="D187" s="3"/>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
-        <v>439</v>
+        <v>446</v>
+      </c>
+      <c r="B188" s="0" t="s">
+        <v>447</v>
       </c>
       <c r="C188" s="5" t="n">
-        <v>2005</v>
+        <v>1985</v>
       </c>
       <c r="D188" s="3"/>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
-        <v>440</v>
+        <v>448</v>
+      </c>
+      <c r="B189" s="0" t="s">
+        <v>449</v>
       </c>
       <c r="C189" s="5" t="n">
+        <v>1995</v>
+      </c>
+      <c r="D189" s="3"/>
+    </row>
+    <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A190" s="0" t="s">
+        <v>450</v>
+      </c>
+      <c r="B190" s="0" t="s">
+        <v>451</v>
+      </c>
+      <c r="C190" s="5" t="n">
         <v>2015</v>
       </c>
-      <c r="D189" s="3"/>
+      <c r="D190" s="3"/>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A191" s="0" t="s">
-        <v>441</v>
-      </c>
-      <c r="B191" s="0" t="s">
-        <v>442</v>
-      </c>
-      <c r="C191" s="5" t="n">
-        <v>2005</v>
-      </c>
+      <c r="C191" s="5"/>
+      <c r="D191" s="3"/>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
-        <v>443</v>
+        <v>452</v>
       </c>
       <c r="B192" s="0" t="s">
-        <v>444</v>
+        <v>453</v>
       </c>
       <c r="C192" s="5" t="n">
+        <v>1965</v>
+      </c>
+      <c r="D192" s="3"/>
+    </row>
+    <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="0" t="s">
+        <v>454</v>
+      </c>
+      <c r="B193" s="0" t="s">
+        <v>455</v>
+      </c>
+      <c r="C193" s="5" t="n">
+        <v>1975</v>
+      </c>
+      <c r="D193" s="3"/>
+    </row>
+    <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A194" s="0" t="s">
+        <v>456</v>
+      </c>
+      <c r="B194" s="0" t="s">
+        <v>457</v>
+      </c>
+      <c r="C194" s="5" t="n">
+        <v>1985</v>
+      </c>
+      <c r="D194" s="3"/>
+    </row>
+    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A195" s="0" t="s">
+        <v>458</v>
+      </c>
+      <c r="B195" s="0" t="s">
+        <v>459</v>
+      </c>
+      <c r="C195" s="5" t="n">
+        <v>2015</v>
+      </c>
+      <c r="D195" s="3"/>
+    </row>
+    <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C196" s="5"/>
+      <c r="D196" s="3"/>
+    </row>
+    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A197" s="0" t="s">
+        <v>460</v>
+      </c>
+      <c r="B197" s="0" t="s">
+        <v>461</v>
+      </c>
+      <c r="C197" s="5" t="n">
+        <v>1975</v>
+      </c>
+      <c r="D197" s="3"/>
+    </row>
+    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A198" s="0" t="s">
+        <v>462</v>
+      </c>
+      <c r="B198" s="0" t="s">
+        <v>463</v>
+      </c>
+      <c r="C198" s="5" t="n">
+        <v>1995</v>
+      </c>
+      <c r="D198" s="3"/>
+    </row>
+    <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A199" s="0" t="s">
+        <v>464</v>
+      </c>
+      <c r="B199" s="0" t="s">
+        <v>465</v>
+      </c>
+      <c r="C199" s="5" t="n">
+        <v>2015</v>
+      </c>
+      <c r="D199" s="3"/>
+    </row>
+    <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C200" s="5"/>
+      <c r="D200" s="3"/>
+    </row>
+    <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="0" t="s">
+        <v>466</v>
+      </c>
+      <c r="C201" s="5" t="n">
+        <v>1965</v>
+      </c>
+      <c r="D201" s="3"/>
+    </row>
+    <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="0" t="s">
+        <v>467</v>
+      </c>
+      <c r="C202" s="5" t="n">
+        <v>1965</v>
+      </c>
+      <c r="D202" s="3" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="0" t="s">
+        <v>469</v>
+      </c>
+      <c r="C203" s="5" t="n">
+        <v>1985</v>
+      </c>
+      <c r="D203" s="3"/>
+    </row>
+    <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A204" s="0" t="s">
+        <v>470</v>
+      </c>
+      <c r="C204" s="5" t="n">
+        <v>2005</v>
+      </c>
+      <c r="D204" s="3"/>
+    </row>
+    <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A205" s="0" t="s">
+        <v>471</v>
+      </c>
+      <c r="C205" s="5" t="n">
+        <v>2015</v>
+      </c>
+      <c r="D205" s="3"/>
+    </row>
+    <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A207" s="0" t="s">
+        <v>472</v>
+      </c>
+      <c r="B207" s="0" t="s">
+        <v>473</v>
+      </c>
+      <c r="C207" s="5" t="n">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A208" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="B208" s="0" t="s">
+        <v>475</v>
+      </c>
+      <c r="C208" s="5" t="n">
         <v>2015</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated Loc for Transport helicopters
Not complete, but a useful guide. 200K Equipment file size milestone :D
</commit_message>
<xml_diff>
--- a/Modding resources/Equipment codes for OOBs.xlsx
+++ b/Modding resources/Equipment codes for OOBs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="497">
   <si>
     <t>Equipment Code</t>
   </si>
@@ -1444,19 +1444,61 @@
     <t>early_helicopter</t>
   </si>
   <si>
+    <t>required for all helicopter research</t>
+  </si>
+  <si>
     <t>attack_helicopter_equipment_1</t>
   </si>
   <si>
+    <t>attack_helicopter1</t>
+  </si>
+  <si>
     <t>Attack Helicopter</t>
   </si>
   <si>
     <t>attack_helicopter_equipment_2</t>
   </si>
   <si>
+    <t>attack_helicopter2</t>
+  </si>
+  <si>
     <t>attack_helicopter_equipment_3</t>
   </si>
   <si>
+    <t>attack_helicopter3</t>
+  </si>
+  <si>
     <t>attack_helicopter_equipment_4</t>
+  </si>
+  <si>
+    <t>attack_helicopter4</t>
+  </si>
+  <si>
+    <t>transport_helicopter_equipment_1</t>
+  </si>
+  <si>
+    <t>transport_helicopter1</t>
+  </si>
+  <si>
+    <t>Transport Helicopter</t>
+  </si>
+  <si>
+    <t>transport_helicopter_equipment_2</t>
+  </si>
+  <si>
+    <t>transport_helicopter2</t>
+  </si>
+  <si>
+    <t>transport_helicopter_equipment_3</t>
+  </si>
+  <si>
+    <t>transport_helicopter3</t>
+  </si>
+  <si>
+    <t>transport_helicopter_equipment_4</t>
+  </si>
+  <si>
+    <t>transport_helicopter4</t>
   </si>
   <si>
     <t>Air_UAV_equipment_1</t>
@@ -1592,23 +1634,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G212"/>
+  <dimension ref="A1:G217"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="510" topLeftCell="A166" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="510" topLeftCell="A190" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B181" activeCellId="0" sqref="B181"/>
+      <selection pane="bottomLeft" activeCell="E215" activeCellId="0" sqref="E215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.4744897959184"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.0255102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.6632653061225"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4220,28 +4261,36 @@
       <c r="D204" s="3"/>
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A205" s="0" t="s">
+      <c r="B205" s="0" t="s">
         <v>473</v>
       </c>
       <c r="C205" s="5" t="n">
         <v>1965</v>
       </c>
-      <c r="D205" s="3"/>
+      <c r="D205" s="3" t="s">
+        <v>474</v>
+      </c>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
-        <v>474</v>
+        <v>475</v>
+      </c>
+      <c r="B206" s="0" t="s">
+        <v>476</v>
       </c>
       <c r="C206" s="5" t="n">
         <v>1965</v>
       </c>
       <c r="D206" s="3" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="s">
-        <v>476</v>
+        <v>478</v>
+      </c>
+      <c r="B207" s="0" t="s">
+        <v>479</v>
       </c>
       <c r="C207" s="5" t="n">
         <v>1985</v>
@@ -4250,7 +4299,10 @@
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="s">
-        <v>477</v>
+        <v>480</v>
+      </c>
+      <c r="B208" s="0" t="s">
+        <v>481</v>
       </c>
       <c r="C208" s="5" t="n">
         <v>2005</v>
@@ -4259,7 +4311,10 @@
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="s">
-        <v>478</v>
+        <v>482</v>
+      </c>
+      <c r="B209" s="0" t="s">
+        <v>483</v>
       </c>
       <c r="C209" s="5" t="n">
         <v>2015</v>
@@ -4268,23 +4323,70 @@
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="s">
-        <v>479</v>
+        <v>484</v>
       </c>
       <c r="B211" s="0" t="s">
-        <v>480</v>
-      </c>
-      <c r="C211" s="5" t="n">
-        <v>2005</v>
+        <v>485</v>
+      </c>
+      <c r="C211" s="0" t="n">
+        <v>1965</v>
+      </c>
+      <c r="D211" s="0" t="s">
+        <v>486</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="s">
-        <v>481</v>
+        <v>487</v>
       </c>
       <c r="B212" s="0" t="s">
-        <v>482</v>
-      </c>
-      <c r="C212" s="5" t="n">
+        <v>488</v>
+      </c>
+      <c r="C212" s="0" t="n">
+        <v>1985</v>
+      </c>
+    </row>
+    <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A213" s="0" t="s">
+        <v>489</v>
+      </c>
+      <c r="B213" s="0" t="s">
+        <v>490</v>
+      </c>
+      <c r="C213" s="0" t="n">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A214" s="0" t="s">
+        <v>491</v>
+      </c>
+      <c r="B214" s="0" t="s">
+        <v>492</v>
+      </c>
+      <c r="C214" s="0" t="n">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A216" s="0" t="s">
+        <v>493</v>
+      </c>
+      <c r="B216" s="0" t="s">
+        <v>494</v>
+      </c>
+      <c r="C216" s="5" t="n">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A217" s="0" t="s">
+        <v>495</v>
+      </c>
+      <c r="B217" s="0" t="s">
+        <v>496</v>
+      </c>
+      <c r="C217" s="5" t="n">
         <v>2015</v>
       </c>
     </row>

</xml_diff>